<commit_message>
Added email notifications to system
</commit_message>
<xml_diff>
--- a/AustinAndHoustonCombinedSalaryGradeInfo.xlsx
+++ b/AustinAndHoustonCombinedSalaryGradeInfo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kinetixhr-my.sharepoint.com/personal/awhelan_kinetixhr_com/Documents/Projects/Opens Projects/TCH/testing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kinetixhr-my.sharepoint.com/personal/awhelan_kinetixhr_com/Documents/Projects/Opens Projects/opensprocessing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{0BB536D3-D32A-426C-BB74-F0FE7600E58F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0271EE6-00B3-459B-9E77-3E0252CC92C5}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="8_{0BB536D3-D32A-426C-BB74-F0FE7600E58F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3492F5ED-A889-4414-978D-7D5A07E5CBE9}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{DFD78DC0-41B0-4334-BF68-8AA421951506}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{DFD78DC0-41B0-4334-BF68-8AA421951506}"/>
   </bookViews>
   <sheets>
     <sheet name="Combined" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="58">
   <si>
     <t>SG</t>
   </si>
@@ -162,9 +162,6 @@
     <t>09</t>
   </si>
   <si>
-    <t>13</t>
-  </si>
-  <si>
     <t>01</t>
   </si>
   <si>
@@ -214,6 +211,27 @@
   </si>
   <si>
     <t>09Austin</t>
+  </si>
+  <si>
+    <t>16EAustin</t>
+  </si>
+  <si>
+    <t>15EAustin</t>
+  </si>
+  <si>
+    <t>11EAustin</t>
+  </si>
+  <si>
+    <t>10EAustin</t>
+  </si>
+  <si>
+    <t>09EAustin</t>
+  </si>
+  <si>
+    <t>08EAustin</t>
+  </si>
+  <si>
+    <t>07EAustin</t>
   </si>
 </sst>
 </file>
@@ -226,7 +244,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -351,6 +369,17 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -634,7 +663,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -770,9 +799,6 @@
     <xf numFmtId="165" fontId="7" fillId="4" borderId="16" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="7" fillId="0" borderId="12" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="7" fillId="4" borderId="12" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -784,6 +810,35 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="17" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="12" xfId="16" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="12" xfId="16" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="10" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="11" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="11" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="12" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="19" fillId="4" borderId="10" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="20" fillId="4" borderId="11" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="19" fillId="4" borderId="11" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="19" fillId="4" borderId="12" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="21">
@@ -1119,20 +1174,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F522DB48-47AD-4BC5-9969-53C6479D82E0}">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1156,1009 +1211,1146 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="87" t="s">
+      <c r="A2" s="91">
+        <v>22</v>
+      </c>
+      <c r="B2" s="5">
+        <v>217963</v>
+      </c>
+      <c r="C2" s="6">
+        <v>254716</v>
+      </c>
+      <c r="D2" s="7">
+        <v>291460</v>
+      </c>
+      <c r="E2" s="6">
+        <v>328203</v>
+      </c>
+      <c r="F2" s="8">
+        <v>364956</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="92">
+        <v>21</v>
+      </c>
+      <c r="B3" s="9">
+        <v>194708</v>
+      </c>
+      <c r="C3" s="10">
+        <v>227489</v>
+      </c>
+      <c r="D3" s="11">
+        <v>260260</v>
+      </c>
+      <c r="E3" s="10">
+        <v>293030</v>
+      </c>
+      <c r="F3" s="12">
+        <v>325811</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="93">
+        <v>20</v>
+      </c>
+      <c r="B4" s="13">
+        <v>173846</v>
+      </c>
+      <c r="C4" s="14">
+        <v>203091</v>
+      </c>
+      <c r="D4" s="15">
+        <v>232336</v>
+      </c>
+      <c r="E4" s="14">
+        <v>261580</v>
+      </c>
+      <c r="F4" s="16">
+        <v>290825</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="92">
+        <v>19</v>
+      </c>
+      <c r="B5" s="9">
+        <v>155105</v>
+      </c>
+      <c r="C5" s="10">
+        <v>181292</v>
+      </c>
+      <c r="D5" s="11">
+        <v>207469</v>
+      </c>
+      <c r="E5" s="10">
+        <v>233646</v>
+      </c>
+      <c r="F5" s="12">
+        <v>259833</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="93">
+        <v>18</v>
+      </c>
+      <c r="B6" s="13">
+        <v>138548</v>
+      </c>
+      <c r="C6" s="14">
+        <v>161907</v>
+      </c>
+      <c r="D6" s="15">
+        <v>185244</v>
+      </c>
+      <c r="E6" s="14">
+        <v>208603</v>
+      </c>
+      <c r="F6" s="16">
+        <v>231940</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="92">
+        <v>17</v>
+      </c>
+      <c r="B7" s="9">
+        <v>123780</v>
+      </c>
+      <c r="C7" s="10">
+        <v>144580</v>
+      </c>
+      <c r="D7" s="11">
+        <v>165391</v>
+      </c>
+      <c r="E7" s="10">
+        <v>186201</v>
+      </c>
+      <c r="F7" s="12">
+        <v>207001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="93">
+        <v>16</v>
+      </c>
+      <c r="B8" s="13">
+        <v>110510</v>
+      </c>
+      <c r="C8" s="14">
+        <v>129105</v>
+      </c>
+      <c r="D8" s="15">
+        <v>147680</v>
+      </c>
+      <c r="E8" s="14">
+        <v>166275</v>
+      </c>
+      <c r="F8" s="16">
+        <v>184849</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="92">
+        <v>15</v>
+      </c>
+      <c r="B9" s="9">
+        <v>98716</v>
+      </c>
+      <c r="C9" s="10">
+        <v>115273</v>
+      </c>
+      <c r="D9" s="11">
+        <v>131840</v>
+      </c>
+      <c r="E9" s="10">
+        <v>148408</v>
+      </c>
+      <c r="F9" s="12">
+        <v>164964</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="94" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="17">
+        <v>88171</v>
+      </c>
+      <c r="C10" s="18">
+        <v>107369</v>
+      </c>
+      <c r="D10" s="19">
+        <v>126568</v>
+      </c>
+      <c r="E10" s="18">
+        <v>145766</v>
+      </c>
+      <c r="F10" s="20">
+        <v>164964</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="92">
+        <v>14</v>
+      </c>
+      <c r="B11" s="9">
+        <v>88171</v>
+      </c>
+      <c r="C11" s="10">
+        <v>102939</v>
+      </c>
+      <c r="D11" s="11">
+        <v>117707</v>
+      </c>
+      <c r="E11" s="10">
+        <v>132475</v>
+      </c>
+      <c r="F11" s="12">
+        <v>147243</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="93" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="13">
+        <v>78665</v>
+      </c>
+      <c r="C12" s="14">
+        <v>95804</v>
+      </c>
+      <c r="D12" s="15">
+        <v>112954</v>
+      </c>
+      <c r="E12" s="14">
+        <v>130104</v>
+      </c>
+      <c r="F12" s="16">
+        <v>147243</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="92">
+        <v>13</v>
+      </c>
+      <c r="B13" s="9">
+        <v>78665</v>
+      </c>
+      <c r="C13" s="10">
+        <v>91873</v>
+      </c>
+      <c r="D13" s="11">
+        <v>105092</v>
+      </c>
+      <c r="E13" s="10">
+        <v>118310</v>
+      </c>
+      <c r="F13" s="12">
+        <v>131518</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="94" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="17">
+        <v>66185</v>
+      </c>
+      <c r="C14" s="18">
+        <v>86444</v>
+      </c>
+      <c r="D14" s="19">
+        <v>106714</v>
+      </c>
+      <c r="E14" s="18">
+        <v>126984</v>
+      </c>
+      <c r="F14" s="20">
+        <v>147243</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="92">
+        <v>12</v>
+      </c>
+      <c r="B15" s="9">
+        <v>70428</v>
+      </c>
+      <c r="C15" s="10">
+        <v>82139</v>
+      </c>
+      <c r="D15" s="11">
+        <v>93849</v>
+      </c>
+      <c r="E15" s="10">
+        <v>105560</v>
+      </c>
+      <c r="F15" s="12">
+        <v>117270</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" thickBot="1">
+      <c r="A16" s="109">
+        <v>11</v>
+      </c>
+      <c r="B16" s="17">
+        <v>63398</v>
+      </c>
+      <c r="C16" s="18">
+        <v>73798</v>
+      </c>
+      <c r="D16" s="19">
+        <v>84198</v>
+      </c>
+      <c r="E16" s="18">
+        <v>94598</v>
+      </c>
+      <c r="F16" s="20">
+        <v>104998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15" thickBot="1">
+      <c r="A17" s="109">
+        <v>10</v>
+      </c>
+      <c r="B17" s="9">
+        <v>57116</v>
+      </c>
+      <c r="C17" s="10">
+        <v>66497</v>
+      </c>
+      <c r="D17" s="11">
+        <v>75857</v>
+      </c>
+      <c r="E17" s="10">
+        <v>85238</v>
+      </c>
+      <c r="F17" s="12">
+        <v>94598</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15" thickBot="1">
+      <c r="A18" s="109" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="17">
+        <v>51376</v>
+      </c>
+      <c r="C18" s="18">
+        <v>59800</v>
+      </c>
+      <c r="D18" s="19">
+        <v>68213</v>
+      </c>
+      <c r="E18" s="18">
+        <v>76627</v>
+      </c>
+      <c r="F18" s="20">
+        <v>85051</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15" thickBot="1">
+      <c r="A19" s="109" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="9">
+        <v>46113</v>
+      </c>
+      <c r="C19" s="10">
+        <v>53705</v>
+      </c>
+      <c r="D19" s="11">
+        <v>61276</v>
+      </c>
+      <c r="E19" s="10">
+        <v>68868</v>
+      </c>
+      <c r="F19" s="12">
+        <v>76440</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15" thickBot="1">
+      <c r="A20" s="109" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="17">
+        <v>41849</v>
+      </c>
+      <c r="C20" s="18">
+        <v>48776</v>
+      </c>
+      <c r="D20" s="19">
+        <v>55712</v>
+      </c>
+      <c r="E20" s="18">
+        <v>62649</v>
+      </c>
+      <c r="F20" s="20">
+        <v>69576</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15" thickBot="1">
+      <c r="A21" s="109" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="9">
+        <v>38084</v>
+      </c>
+      <c r="C21" s="10">
+        <v>44366</v>
+      </c>
+      <c r="D21" s="11">
+        <v>50658</v>
+      </c>
+      <c r="E21" s="10">
+        <v>56950</v>
+      </c>
+      <c r="F21" s="12">
+        <v>63232</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15" thickBot="1">
+      <c r="A22" s="109" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="17">
+        <v>33758</v>
+      </c>
+      <c r="C22" s="18">
+        <v>39998</v>
+      </c>
+      <c r="D22" s="19">
+        <v>46228</v>
+      </c>
+      <c r="E22" s="18">
+        <v>52457</v>
+      </c>
+      <c r="F22" s="20">
+        <v>58697</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15" thickBot="1">
+      <c r="A23" s="109" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="9">
+        <v>33758</v>
+      </c>
+      <c r="C23" s="10">
+        <v>38958</v>
+      </c>
+      <c r="D23" s="11">
+        <v>44168</v>
+      </c>
+      <c r="E23" s="10">
+        <v>49379</v>
+      </c>
+      <c r="F23" s="12">
+        <v>54579</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15" thickBot="1">
+      <c r="A24" s="109" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="17">
+        <v>33758</v>
+      </c>
+      <c r="C24" s="18">
+        <v>38022</v>
+      </c>
+      <c r="D24" s="19">
+        <v>42276</v>
+      </c>
+      <c r="E24" s="18">
+        <v>46529</v>
+      </c>
+      <c r="F24" s="20">
+        <v>50793</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15" thickBot="1">
+      <c r="A25" s="109" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="17">
-        <v>32780</v>
-      </c>
-      <c r="C2" s="18">
-        <v>35256</v>
-      </c>
-      <c r="D2" s="19">
-        <v>37731</v>
-      </c>
-      <c r="E2" s="18">
-        <v>40206</v>
-      </c>
-      <c r="F2" s="20">
-        <v>42681</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="87" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="9">
-        <v>32780</v>
-      </c>
-      <c r="C3" s="10">
-        <v>36046</v>
-      </c>
-      <c r="D3" s="11">
-        <v>39322</v>
-      </c>
-      <c r="E3" s="10">
-        <v>42598</v>
-      </c>
-      <c r="F3" s="12">
-        <v>45864</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="87" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="17">
-        <v>32780</v>
-      </c>
-      <c r="C4" s="18">
-        <v>36920</v>
-      </c>
-      <c r="D4" s="19">
-        <v>41048</v>
-      </c>
-      <c r="E4" s="18">
-        <v>45177</v>
-      </c>
-      <c r="F4" s="20">
-        <v>49316</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="87" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="9">
-        <v>32780</v>
-      </c>
-      <c r="C5" s="10">
-        <v>37835</v>
-      </c>
-      <c r="D5" s="11">
-        <v>42889</v>
-      </c>
-      <c r="E5" s="10">
-        <v>47944</v>
-      </c>
-      <c r="F5" s="12">
-        <v>52998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="87" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="17">
-        <v>32780</v>
-      </c>
-      <c r="C6" s="18">
-        <v>38833</v>
-      </c>
-      <c r="D6" s="19">
-        <v>44886</v>
-      </c>
-      <c r="E6" s="18">
-        <v>50939</v>
-      </c>
-      <c r="F6" s="20">
-        <v>56992</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="87" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="9">
-        <v>36982</v>
-      </c>
-      <c r="C7" s="10">
-        <v>43076</v>
-      </c>
-      <c r="D7" s="11">
-        <v>49181</v>
-      </c>
-      <c r="E7" s="10">
-        <v>55286</v>
-      </c>
-      <c r="F7" s="12">
-        <v>61380</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="87" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="17">
-        <v>40622</v>
-      </c>
-      <c r="C8" s="18">
-        <v>47361</v>
-      </c>
-      <c r="D8" s="19">
-        <v>54090</v>
-      </c>
-      <c r="E8" s="18">
-        <v>60819</v>
-      </c>
-      <c r="F8" s="20">
-        <v>67558</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="87" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="9">
-        <v>44761</v>
-      </c>
-      <c r="C9" s="10">
-        <v>52124</v>
-      </c>
-      <c r="D9" s="11">
-        <v>59488</v>
-      </c>
-      <c r="E9" s="10">
-        <v>66851</v>
-      </c>
-      <c r="F9" s="12">
-        <v>74214</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="87" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="17">
-        <v>49878</v>
-      </c>
-      <c r="C10" s="18">
-        <v>58052</v>
-      </c>
-      <c r="D10" s="19">
-        <v>66227</v>
-      </c>
-      <c r="E10" s="18">
-        <v>74401</v>
-      </c>
-      <c r="F10" s="20">
-        <v>82576</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="87">
-        <v>10</v>
-      </c>
-      <c r="B11" s="9">
-        <v>55452</v>
-      </c>
-      <c r="C11" s="10">
-        <v>64563</v>
-      </c>
-      <c r="D11" s="11">
-        <v>73652</v>
-      </c>
-      <c r="E11" s="10">
-        <v>82763</v>
-      </c>
-      <c r="F11" s="12">
-        <v>91852</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="87">
-        <v>11</v>
-      </c>
-      <c r="B12" s="17">
-        <v>61547</v>
-      </c>
-      <c r="C12" s="18">
-        <v>71656</v>
-      </c>
-      <c r="D12" s="19">
-        <v>81744</v>
-      </c>
-      <c r="E12" s="18">
-        <v>91852</v>
-      </c>
-      <c r="F12" s="20">
-        <v>101940</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="87">
-        <v>12</v>
-      </c>
-      <c r="B13" s="9">
-        <v>68369</v>
-      </c>
-      <c r="C13" s="10">
-        <v>79747</v>
-      </c>
-      <c r="D13" s="11">
-        <v>91114</v>
-      </c>
-      <c r="E13" s="10">
-        <v>102481</v>
-      </c>
-      <c r="F13" s="12">
-        <v>113859</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="87" t="s">
+      <c r="B25" s="9">
+        <v>33758</v>
+      </c>
+      <c r="C25" s="10">
+        <v>37128</v>
+      </c>
+      <c r="D25" s="11">
+        <v>40497</v>
+      </c>
+      <c r="E25" s="10">
+        <v>43867</v>
+      </c>
+      <c r="F25" s="12">
+        <v>47236</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15" thickBot="1">
+      <c r="A26" s="109" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="9">
-        <v>76377</v>
-      </c>
-      <c r="C14" s="10">
-        <v>89211</v>
-      </c>
-      <c r="D14" s="11">
-        <v>102034</v>
-      </c>
-      <c r="E14" s="10">
-        <v>114857</v>
-      </c>
-      <c r="F14" s="12">
-        <v>127691</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="87">
-        <v>14</v>
-      </c>
-      <c r="B15" s="9">
-        <v>85612</v>
-      </c>
-      <c r="C15" s="10">
-        <v>99944</v>
-      </c>
-      <c r="D15" s="11">
-        <v>114285</v>
-      </c>
-      <c r="E15" s="10">
-        <v>128627</v>
-      </c>
-      <c r="F15" s="12">
-        <v>142958</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="87">
-        <v>15</v>
-      </c>
-      <c r="B16" s="9">
-        <v>95846</v>
-      </c>
-      <c r="C16" s="10">
-        <v>111924</v>
-      </c>
-      <c r="D16" s="11">
-        <v>128003</v>
-      </c>
-      <c r="E16" s="10">
-        <v>144081</v>
-      </c>
-      <c r="F16" s="12">
-        <v>160160</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="87">
-        <v>16</v>
-      </c>
-      <c r="B17" s="13">
-        <v>107286</v>
-      </c>
-      <c r="C17" s="14">
-        <v>125340</v>
-      </c>
-      <c r="D17" s="15">
-        <v>143374</v>
-      </c>
-      <c r="E17" s="14">
-        <v>161428</v>
-      </c>
-      <c r="F17" s="16">
-        <v>179462</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="87">
+      <c r="B26" s="95">
+        <v>33758</v>
+      </c>
+      <c r="C26" s="96">
+        <v>36316</v>
+      </c>
+      <c r="D26" s="97">
+        <v>38864</v>
+      </c>
+      <c r="E26" s="96">
+        <v>41412</v>
+      </c>
+      <c r="F26" s="98">
+        <v>43971</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="9">
-        <v>120182</v>
-      </c>
-      <c r="C18" s="10">
-        <v>140379</v>
-      </c>
-      <c r="D18" s="11">
-        <v>160576</v>
-      </c>
-      <c r="E18" s="10">
-        <v>180772</v>
-      </c>
-      <c r="F18" s="12">
-        <v>200969</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="87">
+      <c r="B27" s="43">
+        <v>217963</v>
+      </c>
+      <c r="C27" s="44">
+        <v>254716</v>
+      </c>
+      <c r="D27" s="45">
+        <v>291460</v>
+      </c>
+      <c r="E27" s="44">
+        <v>328203</v>
+      </c>
+      <c r="F27" s="99">
+        <v>364956</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="13">
-        <v>134513</v>
-      </c>
-      <c r="C19" s="14">
-        <v>157185</v>
-      </c>
-      <c r="D19" s="15">
-        <v>179847</v>
-      </c>
-      <c r="E19" s="14">
-        <v>202508</v>
-      </c>
-      <c r="F19" s="16">
-        <v>225180</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="87">
+      <c r="B28" s="52">
+        <v>194708</v>
+      </c>
+      <c r="C28" s="53">
+        <v>227489</v>
+      </c>
+      <c r="D28" s="54">
+        <v>260260</v>
+      </c>
+      <c r="E28" s="53">
+        <v>293030</v>
+      </c>
+      <c r="F28" s="86">
+        <v>325811</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="9">
-        <v>150592</v>
-      </c>
-      <c r="C20" s="10">
-        <v>176009</v>
-      </c>
-      <c r="D20" s="11">
-        <v>201427</v>
-      </c>
-      <c r="E20" s="10">
-        <v>226844</v>
-      </c>
-      <c r="F20" s="12">
-        <v>252262</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="87">
+      <c r="B29" s="61">
+        <v>173846</v>
+      </c>
+      <c r="C29" s="62">
+        <v>203091</v>
+      </c>
+      <c r="D29" s="63">
+        <v>232336</v>
+      </c>
+      <c r="E29" s="62">
+        <v>261580</v>
+      </c>
+      <c r="F29" s="100">
+        <v>290825</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="13">
-        <v>168792</v>
-      </c>
-      <c r="C21" s="14">
-        <v>197184</v>
-      </c>
-      <c r="D21" s="15">
-        <v>225576</v>
-      </c>
-      <c r="E21" s="14">
-        <v>253968</v>
-      </c>
-      <c r="F21" s="16">
-        <v>282360</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="87">
+      <c r="B30" s="52">
+        <v>155105</v>
+      </c>
+      <c r="C30" s="53">
+        <v>181292</v>
+      </c>
+      <c r="D30" s="54">
+        <v>207469</v>
+      </c>
+      <c r="E30" s="53">
+        <v>233646</v>
+      </c>
+      <c r="F30" s="86">
+        <v>259833</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="9">
-        <v>189030</v>
-      </c>
-      <c r="C22" s="10">
-        <v>220854</v>
-      </c>
-      <c r="D22" s="11">
-        <v>252678</v>
-      </c>
-      <c r="E22" s="10">
-        <v>284502</v>
-      </c>
-      <c r="F22" s="12">
-        <v>316326</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="87">
+      <c r="B31" s="61">
+        <v>138548</v>
+      </c>
+      <c r="C31" s="62">
+        <v>161907</v>
+      </c>
+      <c r="D31" s="63">
+        <v>185244</v>
+      </c>
+      <c r="E31" s="62">
+        <v>208603</v>
+      </c>
+      <c r="F31" s="100">
+        <v>231940</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="5">
-        <v>211619</v>
-      </c>
-      <c r="C23" s="6">
-        <v>247291</v>
-      </c>
-      <c r="D23" s="7">
-        <v>282973</v>
-      </c>
-      <c r="E23" s="6">
-        <v>318656</v>
-      </c>
-      <c r="F23" s="8">
-        <v>354328</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="87" t="s">
+      <c r="B32" s="52">
+        <v>123780</v>
+      </c>
+      <c r="C32" s="53">
+        <v>144580</v>
+      </c>
+      <c r="D32" s="54">
+        <v>165391</v>
+      </c>
+      <c r="E32" s="53">
+        <v>186201</v>
+      </c>
+      <c r="F32" s="86">
+        <v>207001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" s="69">
+        <v>110510</v>
+      </c>
+      <c r="C33" s="70">
+        <v>131414</v>
+      </c>
+      <c r="D33" s="71">
+        <v>152301</v>
+      </c>
+      <c r="E33" s="70">
+        <v>173201</v>
+      </c>
+      <c r="F33" s="85">
+        <v>194092</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" s="52">
+        <v>110510</v>
+      </c>
+      <c r="C34" s="53">
+        <v>129105</v>
+      </c>
+      <c r="D34" s="54">
+        <v>147680</v>
+      </c>
+      <c r="E34" s="53">
+        <v>166275</v>
+      </c>
+      <c r="F34" s="86">
+        <v>184849</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" s="69">
+        <v>98716</v>
+      </c>
+      <c r="C35" s="70">
+        <v>117332</v>
+      </c>
+      <c r="D35" s="71">
+        <v>135964</v>
+      </c>
+      <c r="E35" s="70">
+        <v>154585</v>
+      </c>
+      <c r="F35" s="85">
+        <v>173213</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" s="52">
+        <v>98716</v>
+      </c>
+      <c r="C36" s="53">
+        <v>115273</v>
+      </c>
+      <c r="D36" s="54">
+        <v>131840</v>
+      </c>
+      <c r="E36" s="53">
+        <v>148408</v>
+      </c>
+      <c r="F36" s="86">
+        <v>164964</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>25</v>
+      </c>
+      <c r="B37" s="101">
+        <v>88171</v>
+      </c>
+      <c r="C37" s="102">
+        <v>109428</v>
+      </c>
+      <c r="D37" s="103">
+        <v>130692</v>
+      </c>
+      <c r="E37" s="102">
+        <v>151944</v>
+      </c>
+      <c r="F37" s="104">
+        <v>164964</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" s="105">
+        <v>88171</v>
+      </c>
+      <c r="C38" s="106">
+        <v>102939</v>
+      </c>
+      <c r="D38" s="107">
+        <v>117707</v>
+      </c>
+      <c r="E38" s="106">
+        <v>132475</v>
+      </c>
+      <c r="F38" s="108">
+        <v>147243</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" s="101">
+        <v>78665</v>
+      </c>
+      <c r="C39" s="102">
+        <v>97656</v>
+      </c>
+      <c r="D39" s="103">
+        <v>116635</v>
+      </c>
+      <c r="E39" s="102">
+        <v>135616</v>
+      </c>
+      <c r="F39" s="104">
+        <v>147243</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>28</v>
+      </c>
+      <c r="B40" s="105">
+        <v>78665</v>
+      </c>
+      <c r="C40" s="106">
+        <v>91873</v>
+      </c>
+      <c r="D40" s="107">
+        <v>105092</v>
+      </c>
+      <c r="E40" s="106">
+        <v>118310</v>
+      </c>
+      <c r="F40" s="108">
+        <v>131518</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>29</v>
+      </c>
+      <c r="B41" s="101">
+        <v>70428</v>
+      </c>
+      <c r="C41" s="102">
+        <v>88296</v>
+      </c>
+      <c r="D41" s="103">
+        <v>110405</v>
+      </c>
+      <c r="E41" s="102">
+        <v>132496</v>
+      </c>
+      <c r="F41" s="104">
+        <v>131518</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42" s="52">
+        <v>70428</v>
+      </c>
+      <c r="C42" s="53">
+        <v>82139</v>
+      </c>
+      <c r="D42" s="54">
+        <v>93849</v>
+      </c>
+      <c r="E42" s="53">
+        <v>105560</v>
+      </c>
+      <c r="F42" s="86">
+        <v>117270</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>53</v>
+      </c>
+      <c r="B43" s="69">
+        <v>63398</v>
+      </c>
+      <c r="C43" s="70">
+        <v>75108</v>
+      </c>
+      <c r="D43" s="71">
+        <v>86823</v>
+      </c>
+      <c r="E43" s="70">
+        <v>98529</v>
+      </c>
+      <c r="F43" s="85">
+        <v>110248</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
+        <v>31</v>
+      </c>
+      <c r="B44" s="52">
+        <v>63398</v>
+      </c>
+      <c r="C44" s="53">
+        <v>73798</v>
+      </c>
+      <c r="D44" s="54">
+        <v>84198</v>
+      </c>
+      <c r="E44" s="53">
+        <v>94598</v>
+      </c>
+      <c r="F44" s="86">
+        <v>104998</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" t="s">
+        <v>54</v>
+      </c>
+      <c r="B45" s="69">
+        <v>57116</v>
+      </c>
+      <c r="C45" s="70">
+        <v>67662</v>
+      </c>
+      <c r="D45" s="71">
+        <v>78222</v>
+      </c>
+      <c r="E45" s="70">
+        <v>88774</v>
+      </c>
+      <c r="F45" s="85">
+        <v>99328</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="52">
-        <v>55452</v>
-      </c>
-      <c r="C24" s="53">
-        <v>64563</v>
-      </c>
-      <c r="D24" s="54">
-        <v>73652</v>
-      </c>
-      <c r="E24" s="53">
-        <v>82763</v>
-      </c>
-      <c r="F24" s="86">
-        <v>91852</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="87" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" s="69">
-        <v>61547</v>
-      </c>
-      <c r="C25" s="70">
-        <v>71656</v>
-      </c>
-      <c r="D25" s="71">
-        <v>81744</v>
-      </c>
-      <c r="E25" s="70">
-        <v>91852</v>
-      </c>
-      <c r="F25" s="85">
-        <v>101940</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="15" thickBot="1">
-      <c r="A26" s="87" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" s="81">
-        <v>68369</v>
-      </c>
-      <c r="C26" s="82">
-        <v>79747</v>
-      </c>
-      <c r="D26" s="83">
-        <v>91114</v>
-      </c>
-      <c r="E26" s="82">
-        <v>102481</v>
-      </c>
-      <c r="F26" s="84">
-        <v>113859</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="87" t="s">
-        <v>9</v>
-      </c>
-      <c r="B27" s="17">
-        <v>66206</v>
-      </c>
-      <c r="C27" s="18">
-        <v>85404</v>
-      </c>
-      <c r="D27" s="19">
-        <v>104582</v>
-      </c>
-      <c r="E27" s="18">
-        <v>123780</v>
-      </c>
-      <c r="F27" s="19">
-        <v>142958</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="14.5" customHeight="1">
-      <c r="A28" s="87" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" s="69">
-        <v>66206</v>
-      </c>
-      <c r="C28" s="70">
-        <v>85404</v>
-      </c>
-      <c r="D28" s="71">
-        <v>104582</v>
-      </c>
-      <c r="E28" s="70">
-        <v>123780</v>
-      </c>
-      <c r="F28" s="71">
-        <v>142958</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="87" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" s="52">
-        <v>76377</v>
-      </c>
-      <c r="C29" s="53">
-        <v>89211</v>
-      </c>
-      <c r="D29" s="54">
-        <v>102034</v>
-      </c>
-      <c r="E29" s="53">
-        <v>114857</v>
-      </c>
-      <c r="F29" s="54">
-        <v>127691</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="87" t="s">
-        <v>11</v>
-      </c>
-      <c r="B30" s="13">
-        <v>76377</v>
-      </c>
-      <c r="C30" s="14">
-        <v>93017</v>
-      </c>
-      <c r="D30" s="15">
-        <v>109668</v>
-      </c>
-      <c r="E30" s="14">
-        <v>126318</v>
-      </c>
-      <c r="F30" s="15">
-        <v>142958</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="87" t="s">
-        <v>27</v>
-      </c>
-      <c r="B31" s="69">
-        <v>76377</v>
-      </c>
-      <c r="C31" s="70">
-        <v>93017</v>
-      </c>
-      <c r="D31" s="71">
-        <v>109668</v>
-      </c>
-      <c r="E31" s="70">
-        <v>126318</v>
-      </c>
-      <c r="F31" s="71">
-        <v>142958</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="87" t="s">
-        <v>26</v>
-      </c>
-      <c r="B32" s="52">
-        <v>85612</v>
-      </c>
-      <c r="C32" s="53">
-        <v>99944</v>
-      </c>
-      <c r="D32" s="54">
-        <v>114285</v>
-      </c>
-      <c r="E32" s="53">
-        <v>128627</v>
-      </c>
-      <c r="F32" s="54">
-        <v>142958</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="87" t="s">
-        <v>10</v>
-      </c>
-      <c r="B33" s="17">
-        <v>85612</v>
-      </c>
-      <c r="C33" s="18">
-        <v>104249</v>
-      </c>
-      <c r="D33" s="19">
-        <v>122886</v>
-      </c>
-      <c r="E33" s="18">
-        <v>141523</v>
-      </c>
-      <c r="F33" s="19">
-        <v>160160</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="87" t="s">
-        <v>25</v>
-      </c>
-      <c r="B34" s="69">
-        <v>85612</v>
-      </c>
-      <c r="C34" s="70">
-        <v>104249</v>
-      </c>
-      <c r="D34" s="71">
-        <v>122886</v>
-      </c>
-      <c r="E34" s="70">
-        <v>141523</v>
-      </c>
-      <c r="F34" s="71">
-        <v>160160</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="87" t="s">
-        <v>24</v>
-      </c>
-      <c r="B35" s="52">
-        <v>95846</v>
-      </c>
-      <c r="C35" s="53">
-        <v>111924</v>
-      </c>
-      <c r="D35" s="54">
-        <v>128003</v>
-      </c>
-      <c r="E35" s="53">
-        <v>144081</v>
-      </c>
-      <c r="F35" s="54">
-        <v>160160</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="87" t="s">
-        <v>23</v>
-      </c>
-      <c r="B36" s="61">
-        <v>107286</v>
-      </c>
-      <c r="C36" s="62">
-        <v>125340</v>
-      </c>
-      <c r="D36" s="63">
-        <v>143374</v>
-      </c>
-      <c r="E36" s="62">
-        <v>161428</v>
-      </c>
-      <c r="F36" s="63">
-        <v>179462</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="87" t="s">
-        <v>22</v>
-      </c>
-      <c r="B37" s="52">
-        <v>120182</v>
-      </c>
-      <c r="C37" s="53">
-        <v>140379</v>
-      </c>
-      <c r="D37" s="54">
-        <v>160576</v>
-      </c>
-      <c r="E37" s="53">
-        <v>180772</v>
-      </c>
-      <c r="F37" s="54">
-        <v>200969</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="87" t="s">
-        <v>21</v>
-      </c>
-      <c r="B38" s="61">
-        <v>134513</v>
-      </c>
-      <c r="C38" s="62">
-        <v>157185</v>
-      </c>
-      <c r="D38" s="63">
-        <v>179847</v>
-      </c>
-      <c r="E38" s="62">
-        <v>202508</v>
-      </c>
-      <c r="F38" s="63">
-        <v>225180</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="87" t="s">
-        <v>20</v>
-      </c>
-      <c r="B39" s="52">
-        <v>150592</v>
-      </c>
-      <c r="C39" s="53">
-        <v>176009</v>
-      </c>
-      <c r="D39" s="54">
-        <v>201427</v>
-      </c>
-      <c r="E39" s="53">
-        <v>226844</v>
-      </c>
-      <c r="F39" s="54">
-        <v>252262</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="87" t="s">
-        <v>43</v>
-      </c>
-      <c r="B40" s="69">
-        <v>43680</v>
-      </c>
-      <c r="C40" s="70">
-        <v>44200</v>
-      </c>
-      <c r="D40" s="71">
-        <v>44720</v>
-      </c>
-      <c r="E40" s="70">
-        <v>45240</v>
-      </c>
-      <c r="F40" s="71">
-        <v>45760</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="87" t="s">
-        <v>19</v>
-      </c>
-      <c r="B41" s="61">
-        <v>168792</v>
-      </c>
-      <c r="C41" s="62">
-        <v>197184</v>
-      </c>
-      <c r="D41" s="63">
-        <v>225576</v>
-      </c>
-      <c r="E41" s="62">
-        <v>253968</v>
-      </c>
-      <c r="F41" s="63">
-        <v>282360</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42" s="87" t="s">
-        <v>18</v>
-      </c>
-      <c r="B42" s="52">
-        <v>189030</v>
-      </c>
-      <c r="C42" s="53">
-        <v>220854</v>
-      </c>
-      <c r="D42" s="54">
-        <v>252678</v>
-      </c>
-      <c r="E42" s="53">
-        <v>284502</v>
-      </c>
-      <c r="F42" s="54">
-        <v>316326</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="A43" s="87" t="s">
-        <v>17</v>
-      </c>
-      <c r="B43" s="43">
-        <v>211619</v>
-      </c>
-      <c r="C43" s="44">
-        <v>247291</v>
-      </c>
-      <c r="D43" s="45">
-        <v>282973</v>
-      </c>
-      <c r="E43" s="44">
-        <v>318656</v>
-      </c>
-      <c r="F43" s="45">
-        <v>354328</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44" s="87" t="s">
-        <v>44</v>
-      </c>
-      <c r="B44" s="52">
-        <v>43680</v>
-      </c>
-      <c r="C44" s="53">
-        <v>45115</v>
-      </c>
-      <c r="D44" s="54">
-        <v>46540</v>
-      </c>
-      <c r="E44" s="53">
-        <v>47964</v>
-      </c>
-      <c r="F44" s="54">
-        <v>49400</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="A45" s="87" t="s">
-        <v>45</v>
-      </c>
-      <c r="B45" s="69">
-        <v>43680</v>
-      </c>
-      <c r="C45" s="70">
-        <v>46030</v>
-      </c>
-      <c r="D45" s="71">
-        <v>48360</v>
-      </c>
-      <c r="E45" s="70">
-        <v>50710</v>
-      </c>
-      <c r="F45" s="71">
-        <v>53040</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="A46" s="87" t="s">
-        <v>46</v>
-      </c>
       <c r="B46" s="52">
-        <v>43680</v>
+        <v>57116</v>
       </c>
       <c r="C46" s="53">
-        <v>47070</v>
+        <v>66497</v>
       </c>
       <c r="D46" s="54">
-        <v>50440</v>
+        <v>75857</v>
       </c>
       <c r="E46" s="53">
-        <v>53830</v>
-      </c>
-      <c r="F46" s="54">
-        <v>57200</v>
+        <v>85238</v>
+      </c>
+      <c r="F46" s="86">
+        <v>94598</v>
       </c>
     </row>
     <row r="47" spans="1:6">
-      <c r="A47" s="87" t="s">
-        <v>47</v>
+      <c r="A47" t="s">
+        <v>55</v>
       </c>
       <c r="B47" s="69">
-        <v>43680</v>
+        <v>51376</v>
       </c>
       <c r="C47" s="70">
-        <v>48110</v>
+        <v>60860</v>
       </c>
       <c r="D47" s="71">
-        <v>52520</v>
+        <v>70339</v>
       </c>
       <c r="E47" s="70">
-        <v>56950</v>
-      </c>
-      <c r="F47" s="71">
-        <v>61360</v>
+        <v>79830</v>
+      </c>
+      <c r="F47" s="85">
+        <v>89303</v>
       </c>
     </row>
     <row r="48" spans="1:6">
-      <c r="A48" s="87" t="s">
-        <v>48</v>
+      <c r="A48" t="s">
+        <v>50</v>
       </c>
       <c r="B48" s="52">
-        <v>43680</v>
+        <v>51376</v>
       </c>
       <c r="C48" s="53">
-        <v>49275</v>
+        <v>59800</v>
       </c>
       <c r="D48" s="54">
-        <v>54860</v>
+        <v>68213</v>
       </c>
       <c r="E48" s="53">
-        <v>60444</v>
-      </c>
-      <c r="F48" s="54">
-        <v>66040</v>
+        <v>76627</v>
+      </c>
+      <c r="F48" s="86">
+        <v>85051</v>
       </c>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="87" t="s">
+      <c r="A49" t="s">
+        <v>56</v>
+      </c>
+      <c r="B49" s="69">
+        <v>46384</v>
+      </c>
+      <c r="C49" s="70">
+        <v>54849</v>
+      </c>
+      <c r="D49" s="71">
+        <v>63323</v>
+      </c>
+      <c r="E49" s="70">
+        <v>71801</v>
+      </c>
+      <c r="F49" s="85">
+        <v>80262</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" t="s">
         <v>49</v>
-      </c>
-      <c r="B49" s="69">
-        <v>43680</v>
-      </c>
-      <c r="C49" s="70">
-        <v>49649</v>
-      </c>
-      <c r="D49" s="71">
-        <v>55619</v>
-      </c>
-      <c r="E49" s="70">
-        <v>61588</v>
-      </c>
-      <c r="F49" s="71">
-        <v>67558</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
-      <c r="A50" s="87" t="s">
-        <v>50</v>
       </c>
       <c r="B50" s="52">
         <v>46384</v>
       </c>
       <c r="C50" s="53">
-        <v>53352</v>
+        <v>53892</v>
       </c>
       <c r="D50" s="54">
-        <v>60299</v>
+        <v>61412</v>
       </c>
       <c r="E50" s="53">
-        <v>67267</v>
-      </c>
-      <c r="F50" s="54">
-        <v>74214</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="15" thickBot="1">
-      <c r="A51" s="72" t="s">
-        <v>51</v>
-      </c>
-      <c r="B51" s="77">
-        <v>49878</v>
-      </c>
-      <c r="C51" s="78">
-        <v>58052</v>
-      </c>
-      <c r="D51" s="79">
-        <v>66227</v>
-      </c>
-      <c r="E51" s="78">
-        <v>74401</v>
-      </c>
-      <c r="F51" s="79">
-        <v>82576</v>
+        <v>68931</v>
+      </c>
+      <c r="F50" s="86">
+        <v>76440</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" t="s">
+        <v>57</v>
+      </c>
+      <c r="B51" s="69">
+        <v>43680</v>
+      </c>
+      <c r="C51" s="70">
+        <v>51022</v>
+      </c>
+      <c r="D51" s="71">
+        <v>58367</v>
+      </c>
+      <c r="E51" s="70">
+        <v>65707</v>
+      </c>
+      <c r="F51" s="85">
+        <v>73054</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" t="s">
+        <v>48</v>
+      </c>
+      <c r="B52" s="52">
+        <v>43680</v>
+      </c>
+      <c r="C52" s="53">
+        <v>50148</v>
+      </c>
+      <c r="D52" s="54">
+        <v>56628</v>
+      </c>
+      <c r="E52" s="53">
+        <v>63107</v>
+      </c>
+      <c r="F52" s="86">
+        <v>69576</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" t="s">
+        <v>47</v>
+      </c>
+      <c r="B53" s="69">
+        <v>43680</v>
+      </c>
+      <c r="C53" s="70">
+        <v>49275</v>
+      </c>
+      <c r="D53" s="71">
+        <v>54860</v>
+      </c>
+      <c r="E53" s="70">
+        <v>60444</v>
+      </c>
+      <c r="F53" s="85">
+        <v>66040</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" t="s">
+        <v>46</v>
+      </c>
+      <c r="B54" s="52">
+        <v>43680</v>
+      </c>
+      <c r="C54" s="53">
+        <v>48110</v>
+      </c>
+      <c r="D54" s="54">
+        <v>52520</v>
+      </c>
+      <c r="E54" s="53">
+        <v>56950</v>
+      </c>
+      <c r="F54" s="86">
+        <v>61360</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" t="s">
+        <v>45</v>
+      </c>
+      <c r="B55" s="69">
+        <v>43680</v>
+      </c>
+      <c r="C55" s="70">
+        <v>47070</v>
+      </c>
+      <c r="D55" s="71">
+        <v>50440</v>
+      </c>
+      <c r="E55" s="70">
+        <v>53830</v>
+      </c>
+      <c r="F55" s="85">
+        <v>57200</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" t="s">
+        <v>44</v>
+      </c>
+      <c r="B56" s="52">
+        <v>43680</v>
+      </c>
+      <c r="C56" s="53">
+        <v>46030</v>
+      </c>
+      <c r="D56" s="54">
+        <v>48360</v>
+      </c>
+      <c r="E56" s="53">
+        <v>50710</v>
+      </c>
+      <c r="F56" s="86">
+        <v>53040</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" t="s">
+        <v>43</v>
+      </c>
+      <c r="B57" s="69">
+        <v>43680</v>
+      </c>
+      <c r="C57" s="70">
+        <v>45115</v>
+      </c>
+      <c r="D57" s="71">
+        <v>46540</v>
+      </c>
+      <c r="E57" s="70">
+        <v>47964</v>
+      </c>
+      <c r="F57" s="85">
+        <v>49400</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="15" thickBot="1">
+      <c r="A58" t="s">
+        <v>42</v>
+      </c>
+      <c r="B58" s="81">
+        <v>43680</v>
+      </c>
+      <c r="C58" s="82">
+        <v>44200</v>
+      </c>
+      <c r="D58" s="83">
+        <v>44720</v>
+      </c>
+      <c r="E58" s="82">
+        <v>45240</v>
+      </c>
+      <c r="F58" s="84">
+        <v>45760</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F51">
-    <sortCondition ref="A1:A51"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2171,13 +2363,13 @@
       <selection activeCell="B31" sqref="B5:L31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="8" max="8" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:14">
@@ -2246,22 +2438,22 @@
       <c r="M4" s="28"/>
       <c r="N4" s="28"/>
     </row>
-    <row r="5" spans="2:14" ht="16" thickBot="1">
+    <row r="5" spans="2:14" ht="16.2" thickBot="1">
       <c r="B5" s="32"/>
-      <c r="C5" s="88" t="s">
+      <c r="C5" s="87" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="89"/>
-      <c r="E5" s="89"/>
-      <c r="F5" s="89"/>
-      <c r="G5" s="90"/>
-      <c r="H5" s="88" t="s">
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="89"/>
+      <c r="H5" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="89"/>
-      <c r="J5" s="89"/>
-      <c r="K5" s="89"/>
-      <c r="L5" s="90"/>
+      <c r="I5" s="88"/>
+      <c r="J5" s="88"/>
+      <c r="K5" s="88"/>
+      <c r="L5" s="89"/>
       <c r="M5" s="28"/>
       <c r="N5" s="28"/>
     </row>
@@ -3261,32 +3453,32 @@
       <c r="N32" s="28"/>
     </row>
     <row r="33" spans="2:12">
-      <c r="B33" s="91" t="s">
+      <c r="B33" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="C33" s="91"/>
-      <c r="D33" s="91"/>
-      <c r="E33" s="91"/>
-      <c r="F33" s="91"/>
-      <c r="G33" s="91"/>
-      <c r="H33" s="91"/>
-      <c r="I33" s="91"/>
-      <c r="J33" s="91"/>
-      <c r="K33" s="91"/>
-      <c r="L33" s="91"/>
+      <c r="C33" s="90"/>
+      <c r="D33" s="90"/>
+      <c r="E33" s="90"/>
+      <c r="F33" s="90"/>
+      <c r="G33" s="90"/>
+      <c r="H33" s="90"/>
+      <c r="I33" s="90"/>
+      <c r="J33" s="90"/>
+      <c r="K33" s="90"/>
+      <c r="L33" s="90"/>
     </row>
     <row r="34" spans="2:12">
-      <c r="B34" s="91"/>
-      <c r="C34" s="91"/>
-      <c r="D34" s="91"/>
-      <c r="E34" s="91"/>
-      <c r="F34" s="91"/>
-      <c r="G34" s="91"/>
-      <c r="H34" s="91"/>
-      <c r="I34" s="91"/>
-      <c r="J34" s="91"/>
-      <c r="K34" s="91"/>
-      <c r="L34" s="91"/>
+      <c r="B34" s="90"/>
+      <c r="C34" s="90"/>
+      <c r="D34" s="90"/>
+      <c r="E34" s="90"/>
+      <c r="F34" s="90"/>
+      <c r="G34" s="90"/>
+      <c r="H34" s="90"/>
+      <c r="I34" s="90"/>
+      <c r="J34" s="90"/>
+      <c r="K34" s="90"/>
+      <c r="L34" s="90"/>
     </row>
     <row r="35" spans="2:12">
       <c r="B35" s="32"/>
@@ -3301,7 +3493,7 @@
       <c r="K35" s="28"/>
       <c r="L35" s="28"/>
     </row>
-    <row r="36" spans="2:12" ht="15.5">
+    <row r="36" spans="2:12" ht="15">
       <c r="B36" s="21" t="s">
         <v>8</v>
       </c>

</xml_diff>